<commit_message>
Adding URL validation for login test case
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20424" windowHeight="4428"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16452" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>